<commit_message>
Do not check processed elements, add regex back to basic emoticons
</commit_message>
<xml_diff>
--- a/emoList.xlsx
+++ b/emoList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvh/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvh/Dropbox/Programing/Chrome Extension/Facebook Emoticons/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$1:$G$137</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="233">
   <si>
     <t>:)</t>
   </si>
@@ -720,6 +723,12 @@
   </si>
   <si>
     <t>Yahoo messenger 11 hidden emo</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>cant</t>
   </si>
 </sst>
 </file>
@@ -7503,13 +7512,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="F114" sqref="F100:F114"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -7517,8 +7526,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -7526,8 +7538,11 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -7535,8 +7550,11 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -7544,8 +7562,11 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -7554,7 +7575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -7563,7 +7584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -7571,8 +7592,11 @@
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>14</v>
@@ -7580,8 +7604,11 @@
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>16</v>
@@ -7590,7 +7617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>18</v>
@@ -7598,8 +7625,11 @@
       <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>20</v>
@@ -7607,8 +7637,11 @@
       <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>22</v>
@@ -7617,7 +7650,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>24</v>
@@ -7625,8 +7658,11 @@
       <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>26</v>
@@ -7635,7 +7671,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>28</v>
@@ -7643,8 +7679,11 @@
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>30</v>
@@ -7652,8 +7691,11 @@
       <c r="C16" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
         <v>32</v>
@@ -7661,8 +7703,11 @@
       <c r="C17" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
         <v>34</v>
@@ -7671,7 +7716,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
         <v>36</v>
@@ -7680,7 +7725,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
         <v>38</v>
@@ -7689,7 +7734,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
         <v>40</v>
@@ -7698,7 +7743,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
         <v>42</v>
@@ -7706,8 +7751,11 @@
       <c r="C22" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
         <v>44</v>
@@ -7716,7 +7764,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>46</v>
@@ -7725,7 +7773,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
         <v>48</v>
@@ -7734,7 +7782,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>50</v>
@@ -7743,7 +7791,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
         <v>52</v>
@@ -7752,7 +7800,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
         <v>65</v>
@@ -7761,7 +7809,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
         <v>67</v>
@@ -7770,7 +7818,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
         <v>69</v>
@@ -7779,7 +7827,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
         <v>71</v>
@@ -7788,7 +7836,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
         <v>73</v>
@@ -7797,7 +7845,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
         <v>74</v>
@@ -7806,7 +7854,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
         <v>76</v>
@@ -7815,7 +7863,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
         <v>78</v>
@@ -7824,7 +7872,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
         <v>80</v>
@@ -7833,7 +7881,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
         <v>82</v>
@@ -7842,7 +7890,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
         <v>84</v>
@@ -7851,7 +7899,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2" t="s">
         <v>86</v>
@@ -7860,7 +7908,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
         <v>88</v>
@@ -7869,7 +7917,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
         <v>89</v>
@@ -7878,7 +7926,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
@@ -7887,7 +7935,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
         <v>93</v>
@@ -7896,7 +7944,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
         <v>95</v>
@@ -7905,7 +7953,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2" t="s">
         <v>97</v>
@@ -7914,7 +7962,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2" t="s">
         <v>99</v>
@@ -7922,8 +7970,11 @@
       <c r="C46" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2" t="s">
         <v>101</v>
@@ -7932,7 +7983,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2" t="s">
         <v>103</v>
@@ -8583,6 +8634,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="G1:G137"/>
   <mergeCells count="1">
     <mergeCell ref="E116:H116"/>
   </mergeCells>

</xml_diff>

<commit_message>
remove onAction events, clean up code, turn on log
</commit_message>
<xml_diff>
--- a/emoList.xlsx
+++ b/emoList.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="264">
   <si>
     <t>:)</t>
   </si>
@@ -729,13 +729,106 @@
   </si>
   <si>
     <t>cant</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>~</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -776,6 +869,32 @@
       <color rgb="FF666666"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF252525"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF0B0080"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -798,7 +917,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -809,6 +928,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7510,15 +7636,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:R137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -7530,7 +7656,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -7541,8 +7667,9 @@
       <c r="G2" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -7554,7 +7681,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -7565,8 +7692,14 @@
       <c r="G4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K4" s="4"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -7574,8 +7707,14 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K5" s="10"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="12"/>
+    </row>
+    <row r="6" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -7583,8 +7722,14 @@
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K6" s="10"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -7595,8 +7740,14 @@
       <c r="G7" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K7" s="10"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="12"/>
+    </row>
+    <row r="8" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>14</v>
@@ -7607,8 +7758,13 @@
       <c r="G8" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>16</v>
@@ -7616,8 +7772,13 @@
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>18</v>
@@ -7628,8 +7789,16 @@
       <c r="G10" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="9"/>
+      <c r="R10" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>20</v>
@@ -7640,8 +7809,16 @@
       <c r="G11" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="9"/>
+      <c r="R11" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>22</v>
@@ -7649,8 +7826,16 @@
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="9"/>
+      <c r="R12" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>24</v>
@@ -7661,8 +7846,16 @@
       <c r="G13" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="9"/>
+      <c r="R13" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>26</v>
@@ -7670,8 +7863,16 @@
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="9"/>
+      <c r="R14" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>28</v>
@@ -7682,8 +7883,16 @@
       <c r="G15" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="9"/>
+      <c r="R15" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>30</v>
@@ -7694,8 +7903,16 @@
       <c r="G16" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="9"/>
+      <c r="R16" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
         <v>32</v>
@@ -7706,8 +7923,16 @@
       <c r="G17" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="9"/>
+      <c r="R17" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
         <v>34</v>
@@ -7715,8 +7940,16 @@
       <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="9"/>
+      <c r="R18" s="9" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
         <v>36</v>
@@ -7724,8 +7957,16 @@
       <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="9"/>
+      <c r="R19" s="9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
         <v>38</v>
@@ -7733,8 +7974,16 @@
       <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="9"/>
+      <c r="R20" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
         <v>40</v>
@@ -7742,8 +7991,16 @@
       <c r="C21" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="9"/>
+      <c r="R21" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
         <v>42</v>
@@ -7754,8 +8011,16 @@
       <c r="G22" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="9"/>
+      <c r="R22" s="9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
         <v>44</v>
@@ -7763,8 +8028,17 @@
       <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K23" s="10"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="12"/>
+      <c r="R23" s="9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>46</v>
@@ -7772,8 +8046,17 @@
       <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K24" s="10"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="12"/>
+      <c r="R24" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
         <v>48</v>
@@ -7781,8 +8064,16 @@
       <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="9"/>
+      <c r="R25" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>50</v>
@@ -7790,8 +8081,16 @@
       <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="9"/>
+      <c r="R26" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
         <v>52</v>
@@ -7799,8 +8098,16 @@
       <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="9"/>
+      <c r="R27" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
         <v>65</v>
@@ -7808,8 +8115,16 @@
       <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="9"/>
+      <c r="R28" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
         <v>67</v>
@@ -7817,8 +8132,16 @@
       <c r="C29" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="9"/>
+      <c r="R29" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
         <v>69</v>
@@ -7826,8 +8149,16 @@
       <c r="C30" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="9"/>
+      <c r="R30" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
         <v>71</v>
@@ -7835,8 +8166,16 @@
       <c r="C31" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="9"/>
+      <c r="R31" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
         <v>73</v>
@@ -7844,8 +8183,16 @@
       <c r="C32" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="9"/>
+      <c r="R32" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
         <v>74</v>
@@ -7853,8 +8200,16 @@
       <c r="C33" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="9"/>
+      <c r="R33" s="9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
         <v>76</v>
@@ -7862,8 +8217,17 @@
       <c r="C34" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K34" s="10"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="12"/>
+      <c r="R34" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
         <v>78</v>
@@ -7871,8 +8235,17 @@
       <c r="C35" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K35" s="10"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="12"/>
+      <c r="R35" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
         <v>80</v>
@@ -7880,8 +8253,17 @@
       <c r="C36" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K36" s="10"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="12"/>
+      <c r="R36" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
         <v>82</v>
@@ -7889,8 +8271,16 @@
       <c r="C37" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="9"/>
+      <c r="R37" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="2" t="s">
         <v>84</v>
@@ -7898,8 +8288,16 @@
       <c r="C38" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="9"/>
+      <c r="R38" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="2" t="s">
         <v>86</v>
@@ -7907,8 +8305,16 @@
       <c r="C39" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="9"/>
+      <c r="R39" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="2" t="s">
         <v>88</v>
@@ -7916,8 +8322,16 @@
       <c r="C40" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="9"/>
+      <c r="R40" s="12" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="2" t="s">
         <v>89</v>
@@ -7925,8 +8339,14 @@
       <c r="C41" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="9"/>
+      <c r="R41" s="12"/>
+    </row>
+    <row r="42" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="2" t="s">
         <v>91</v>
@@ -7934,8 +8354,14 @@
       <c r="C42" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="9"/>
+      <c r="R42" s="12"/>
+    </row>
+    <row r="43" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
         <v>93</v>
@@ -7943,8 +8369,14 @@
       <c r="C43" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K43" s="10"/>
+      <c r="L43" s="12"/>
+      <c r="M43" s="12"/>
+      <c r="N43" s="12"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="12"/>
+    </row>
+    <row r="44" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="2" t="s">
         <v>95</v>
@@ -7952,8 +8384,14 @@
       <c r="C44" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K44" s="10"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="14"/>
+      <c r="P44" s="12"/>
+    </row>
+    <row r="45" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="2" t="s">
         <v>97</v>
@@ -7961,8 +8399,14 @@
       <c r="C45" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K45" s="10"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="14"/>
+      <c r="P45" s="12"/>
+    </row>
+    <row r="46" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2" t="s">
         <v>99</v>
@@ -7973,8 +8417,13 @@
       <c r="G46" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="9"/>
+    </row>
+    <row r="47" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="2" t="s">
         <v>101</v>
@@ -7982,8 +8431,13 @@
       <c r="C47" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="9"/>
+    </row>
+    <row r="48" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="2" t="s">
         <v>103</v>
@@ -7991,8 +8445,13 @@
       <c r="C48" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="9"/>
+    </row>
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="2" t="s">
         <v>125</v>
@@ -8000,8 +8459,13 @@
       <c r="C49" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="9"/>
+    </row>
+    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2" t="s">
         <v>127</v>
@@ -8009,8 +8473,13 @@
       <c r="C50" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="9"/>
+    </row>
+    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="2" t="s">
         <v>129</v>
@@ -8018,8 +8487,13 @@
       <c r="C51" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="9"/>
+    </row>
+    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="2" t="s">
         <v>131</v>
@@ -8027,8 +8501,13 @@
       <c r="C52" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="9"/>
+    </row>
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="2" t="s">
         <v>133</v>
@@ -8036,8 +8515,13 @@
       <c r="C53" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="9"/>
+    </row>
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="2" t="s">
         <v>135</v>
@@ -8045,8 +8529,13 @@
       <c r="C54" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="9"/>
+    </row>
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="2" t="s">
         <v>137</v>
@@ -8054,8 +8543,13 @@
       <c r="C55" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="9"/>
+    </row>
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="2" t="s">
         <v>139</v>
@@ -8063,8 +8557,13 @@
       <c r="C56" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="9"/>
+    </row>
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2" t="s">
         <v>141</v>
@@ -8072,8 +8571,13 @@
       <c r="C57" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="9"/>
+    </row>
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="2" t="s">
         <v>143</v>
@@ -8081,8 +8585,13 @@
       <c r="C58" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="9"/>
+    </row>
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="2" t="s">
         <v>145</v>
@@ -8090,8 +8599,13 @@
       <c r="C59" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="9"/>
+    </row>
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2" t="s">
         <v>147</v>
@@ -8099,8 +8613,13 @@
       <c r="C60" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="9"/>
+    </row>
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2" t="s">
         <v>149</v>
@@ -8108,8 +8627,13 @@
       <c r="C61" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="9"/>
+    </row>
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="2" t="s">
         <v>151</v>
@@ -8117,8 +8641,13 @@
       <c r="C62" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="9"/>
+    </row>
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="2" t="s">
         <v>153</v>
@@ -8126,8 +8655,13 @@
       <c r="C63" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="9"/>
+    </row>
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="2" t="s">
         <v>155</v>
@@ -8135,8 +8669,13 @@
       <c r="C64" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="9"/>
+    </row>
+    <row r="65" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="2" t="s">
         <v>157</v>
@@ -8144,8 +8683,13 @@
       <c r="C65" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="9"/>
+    </row>
+    <row r="66" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
         <v>159</v>
@@ -8153,8 +8697,13 @@
       <c r="C66" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="9"/>
+    </row>
+    <row r="67" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="2" t="s">
         <v>161</v>
@@ -8162,8 +8711,13 @@
       <c r="C67" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="9"/>
+    </row>
+    <row r="68" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="2" t="s">
         <v>163</v>
@@ -8171,8 +8725,13 @@
       <c r="C68" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="9"/>
+    </row>
+    <row r="69" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="2" t="s">
         <v>165</v>
@@ -8180,8 +8739,13 @@
       <c r="C69" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="9"/>
+    </row>
+    <row r="70" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
         <v>167</v>
@@ -8189,8 +8753,13 @@
       <c r="C70" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="9"/>
+    </row>
+    <row r="71" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="2" t="s">
         <v>169</v>
@@ -8198,8 +8767,14 @@
       <c r="C71" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K71" s="10"/>
+      <c r="L71" s="12"/>
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+      <c r="O71" s="14"/>
+      <c r="P71" s="12"/>
+    </row>
+    <row r="72" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="2" t="s">
         <v>178</v>
@@ -8207,8 +8782,14 @@
       <c r="C72" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K72" s="10"/>
+      <c r="L72" s="12"/>
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="14"/>
+      <c r="P72" s="12"/>
+    </row>
+    <row r="73" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="2" t="s">
         <v>121</v>
@@ -8216,8 +8797,14 @@
       <c r="C73" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K73" s="10"/>
+      <c r="L73" s="12"/>
+      <c r="M73" s="12"/>
+      <c r="N73" s="12"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="12"/>
+    </row>
+    <row r="74" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2" t="s">
         <v>181</v>
@@ -8225,8 +8812,13 @@
       <c r="C74" s="1" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K74" s="9"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="9"/>
+    </row>
+    <row r="75" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="2" t="s">
         <v>183</v>
@@ -8234,8 +8826,13 @@
       <c r="C75" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K75" s="9"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="9"/>
+    </row>
+    <row r="76" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="2" t="s">
         <v>171</v>
@@ -8243,8 +8840,13 @@
       <c r="C76" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="9"/>
+    </row>
+    <row r="77" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="2" t="s">
         <v>173</v>
@@ -8252,8 +8854,13 @@
       <c r="C77" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="9"/>
+    </row>
+    <row r="78" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="2" t="s">
         <v>120</v>
@@ -8261,8 +8868,13 @@
       <c r="C78" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="9"/>
+    </row>
+    <row r="79" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="2" t="s">
         <v>176</v>
@@ -8270,38 +8882,174 @@
       <c r="C79" s="1" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K79" s="10"/>
+      <c r="L79" s="12"/>
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
+      <c r="O79" s="12"/>
+      <c r="P79" s="12"/>
+    </row>
+    <row r="80" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K80" s="10"/>
+      <c r="L80" s="12"/>
+      <c r="M80" s="12"/>
+      <c r="N80" s="12"/>
+      <c r="O80" s="12"/>
+      <c r="P80" s="12"/>
+    </row>
+    <row r="81" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K81" s="10"/>
+      <c r="L81" s="12"/>
+      <c r="M81" s="12"/>
+      <c r="N81" s="12"/>
+      <c r="O81" s="12"/>
+      <c r="P81" s="12"/>
+    </row>
+    <row r="82" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="9"/>
+      <c r="O82" s="9"/>
+    </row>
+    <row r="83" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K83" s="9"/>
+      <c r="L83" s="9"/>
+      <c r="M83" s="9"/>
+      <c r="N83" s="9"/>
+      <c r="O83" s="9"/>
+    </row>
+    <row r="84" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K84" s="9"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="9"/>
+      <c r="O84" s="9"/>
+    </row>
+    <row r="85" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="9"/>
+      <c r="O85" s="9"/>
+    </row>
+    <row r="86" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="C86" s="1"/>
-    </row>
-    <row r="95" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K86" s="9"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="9"/>
+      <c r="N86" s="9"/>
+      <c r="O86" s="9"/>
+    </row>
+    <row r="87" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="9"/>
+      <c r="N87" s="9"/>
+      <c r="O87" s="9"/>
+    </row>
+    <row r="88" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="9"/>
+      <c r="N88" s="9"/>
+      <c r="O88" s="9"/>
+    </row>
+    <row r="89" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K89" s="9"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="9"/>
+      <c r="N89" s="9"/>
+      <c r="O89" s="9"/>
+    </row>
+    <row r="90" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K90" s="9"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="9"/>
+      <c r="O90" s="9"/>
+    </row>
+    <row r="91" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K91" s="9"/>
+      <c r="L91" s="9"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="9"/>
+      <c r="O91" s="9"/>
+    </row>
+    <row r="92" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K92" s="9"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="9"/>
+      <c r="O92" s="9"/>
+    </row>
+    <row r="93" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K93" s="9"/>
+      <c r="L93" s="9"/>
+      <c r="M93" s="9"/>
+      <c r="N93" s="9"/>
+      <c r="O93" s="9"/>
+    </row>
+    <row r="94" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K94" s="9"/>
+      <c r="L94" s="9"/>
+      <c r="M94" s="9"/>
+      <c r="N94" s="9"/>
+      <c r="O94" s="9"/>
+    </row>
+    <row r="95" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K95" s="9"/>
+      <c r="L95" s="9"/>
+      <c r="M95" s="9"/>
+      <c r="N95" s="9"/>
+      <c r="O95" s="9"/>
+    </row>
+    <row r="96" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="C96" s="1"/>
-    </row>
-    <row r="97" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K96" s="9"/>
+      <c r="L96" s="9"/>
+      <c r="M96" s="9"/>
+      <c r="N96" s="9"/>
+      <c r="O96" s="9"/>
+    </row>
+    <row r="97" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="C97" s="1"/>
-    </row>
-    <row r="100" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K97" s="9"/>
+      <c r="L97" s="9"/>
+      <c r="M97" s="9"/>
+      <c r="N97" s="9"/>
+      <c r="O97" s="9"/>
+    </row>
+    <row r="98" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K98" s="9"/>
+      <c r="L98" s="9"/>
+      <c r="M98" s="9"/>
+      <c r="N98" s="9"/>
+      <c r="O98" s="9"/>
+    </row>
+    <row r="99" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+      <c r="K99" s="9"/>
+      <c r="L99" s="9"/>
+      <c r="M99" s="9"/>
+      <c r="N99" s="9"/>
+      <c r="O99" s="9"/>
+    </row>
+    <row r="100" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="2" t="s">
         <v>56</v>
@@ -8309,8 +9057,13 @@
       <c r="C100" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K100" s="9"/>
+      <c r="L100" s="9"/>
+      <c r="M100" s="9"/>
+      <c r="N100" s="9"/>
+      <c r="O100" s="9"/>
+    </row>
+    <row r="101" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="2" t="s">
         <v>54</v>
@@ -8318,8 +9071,13 @@
       <c r="C101" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K101" s="9"/>
+      <c r="L101" s="9"/>
+      <c r="M101" s="9"/>
+      <c r="N101" s="9"/>
+      <c r="O101" s="9"/>
+    </row>
+    <row r="102" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="2" t="s">
         <v>58</v>
@@ -8327,8 +9085,13 @@
       <c r="C102" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K102" s="9"/>
+      <c r="L102" s="9"/>
+      <c r="M102" s="9"/>
+      <c r="N102" s="9"/>
+      <c r="O102" s="9"/>
+    </row>
+    <row r="103" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="2" t="s">
         <v>59</v>
@@ -8336,8 +9099,13 @@
       <c r="C103" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K103" s="9"/>
+      <c r="L103" s="9"/>
+      <c r="M103" s="9"/>
+      <c r="N103" s="9"/>
+      <c r="O103" s="9"/>
+    </row>
+    <row r="104" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="2" t="s">
         <v>61</v>
@@ -8345,8 +9113,13 @@
       <c r="C104" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K104" s="9"/>
+      <c r="L104" s="9"/>
+      <c r="M104" s="9"/>
+      <c r="N104" s="9"/>
+      <c r="O104" s="9"/>
+    </row>
+    <row r="105" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="2" t="s">
         <v>63</v>
@@ -8354,23 +9127,45 @@
       <c r="C105" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" ht="22" x14ac:dyDescent="0.3">
+      <c r="K105" s="9"/>
+      <c r="L105" s="9"/>
+      <c r="M105" s="9"/>
+      <c r="N105" s="9"/>
+      <c r="O105" s="9"/>
+    </row>
+    <row r="106" spans="1:16" ht="22" x14ac:dyDescent="0.3">
       <c r="B106" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" ht="22" x14ac:dyDescent="0.3">
+      <c r="K106" s="9"/>
+      <c r="L106" s="9"/>
+      <c r="M106" s="9"/>
+      <c r="N106" s="9"/>
+      <c r="O106" s="9"/>
+    </row>
+    <row r="107" spans="1:16" ht="22" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="K107" s="10"/>
+      <c r="L107" s="12"/>
+      <c r="M107" s="12"/>
+      <c r="N107" s="12"/>
+      <c r="O107" s="14"/>
+      <c r="P107" s="12"/>
+    </row>
+    <row r="108" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K108" s="10"/>
+      <c r="L108" s="12"/>
+      <c r="M108" s="12"/>
+      <c r="N108" s="12"/>
+      <c r="O108" s="14"/>
+      <c r="P108" s="12"/>
+    </row>
+    <row r="109" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="2" t="s">
         <v>105</v>
@@ -8378,8 +9173,14 @@
       <c r="C109" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K109" s="10"/>
+      <c r="L109" s="12"/>
+      <c r="M109" s="12"/>
+      <c r="N109" s="12"/>
+      <c r="O109" s="14"/>
+      <c r="P109" s="12"/>
+    </row>
+    <row r="110" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="2" t="s">
         <v>106</v>
@@ -8387,8 +9188,13 @@
       <c r="C110" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K110" s="9"/>
+      <c r="L110" s="9"/>
+      <c r="M110" s="9"/>
+      <c r="N110" s="4"/>
+      <c r="O110" s="9"/>
+    </row>
+    <row r="111" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="2" t="s">
         <v>108</v>
@@ -8396,8 +9202,13 @@
       <c r="C111" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="K111" s="9"/>
+      <c r="L111" s="9"/>
+      <c r="M111" s="9"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="9"/>
+    </row>
+    <row r="112" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="2" t="s">
         <v>110</v>
@@ -8405,6 +9216,11 @@
       <c r="C112" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="K112" s="9"/>
+      <c r="L112" s="9"/>
+      <c r="M112" s="9"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="9"/>
     </row>
     <row r="113" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>

</xml_diff>

<commit_message>
change changelog in readme, add :)) and :(( as basic, fix cannot run
</commit_message>
<xml_diff>
--- a/emoList.xlsx
+++ b/emoList.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="264">
   <si>
     <t>:)</t>
   </si>
@@ -925,9 +925,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -935,6 +932,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7638,8 +7638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7667,7 +7667,7 @@
       <c r="G2" t="s">
         <v>231</v>
       </c>
-      <c r="K2" s="8"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -7693,11 +7693,11 @@
         <v>231</v>
       </c>
       <c r="K4" s="4"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
     </row>
     <row r="5" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -7707,12 +7707,12 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="12"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -7722,12 +7722,12 @@
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="12"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="11"/>
     </row>
     <row r="7" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -7740,12 +7740,12 @@
       <c r="G7" t="s">
         <v>232</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="12"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="11"/>
     </row>
     <row r="8" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -7758,11 +7758,11 @@
       <c r="G8" t="s">
         <v>231</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
       <c r="N8" s="4"/>
-      <c r="O8" s="9"/>
+      <c r="O8" s="8"/>
     </row>
     <row r="9" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -7772,11 +7772,11 @@
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="9"/>
+      <c r="O9" s="8"/>
     </row>
     <row r="10" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -7789,12 +7789,12 @@
       <c r="G10" t="s">
         <v>231</v>
       </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="9"/>
-      <c r="R10" s="9" t="s">
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="8"/>
+      <c r="R10" s="8" t="s">
         <v>234</v>
       </c>
     </row>
@@ -7809,12 +7809,12 @@
       <c r="G11" t="s">
         <v>231</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="9"/>
-      <c r="R11" s="9" t="s">
+      <c r="O11" s="8"/>
+      <c r="R11" s="8" t="s">
         <v>235</v>
       </c>
     </row>
@@ -7826,12 +7826,12 @@
       <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="9"/>
-      <c r="R12" s="9" t="s">
+      <c r="O12" s="8"/>
+      <c r="R12" s="8" t="s">
         <v>233</v>
       </c>
     </row>
@@ -7846,12 +7846,12 @@
       <c r="G13" t="s">
         <v>231</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="9"/>
-      <c r="R13" s="9" t="s">
+      <c r="O13" s="8"/>
+      <c r="R13" s="8" t="s">
         <v>236</v>
       </c>
     </row>
@@ -7863,12 +7863,12 @@
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="9"/>
-      <c r="R14" s="9" t="s">
+      <c r="O14" s="8"/>
+      <c r="R14" s="8" t="s">
         <v>237</v>
       </c>
     </row>
@@ -7883,12 +7883,12 @@
       <c r="G15" t="s">
         <v>231</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="9"/>
-      <c r="R15" s="9" t="s">
+      <c r="O15" s="8"/>
+      <c r="R15" s="8" t="s">
         <v>238</v>
       </c>
     </row>
@@ -7903,12 +7903,12 @@
       <c r="G16" t="s">
         <v>231</v>
       </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="9"/>
-      <c r="R16" s="9" t="s">
+      <c r="O16" s="8"/>
+      <c r="R16" s="8" t="s">
         <v>239</v>
       </c>
     </row>
@@ -7923,12 +7923,12 @@
       <c r="G17" t="s">
         <v>231</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="9"/>
-      <c r="R17" s="9" t="s">
+      <c r="O17" s="8"/>
+      <c r="R17" s="8" t="s">
         <v>240</v>
       </c>
     </row>
@@ -7940,12 +7940,12 @@
       <c r="C18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="9"/>
-      <c r="R18" s="9" t="s">
+      <c r="O18" s="8"/>
+      <c r="R18" s="8" t="s">
         <v>241</v>
       </c>
     </row>
@@ -7957,12 +7957,12 @@
       <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="9"/>
-      <c r="R19" s="9" t="s">
+      <c r="O19" s="8"/>
+      <c r="R19" s="8" t="s">
         <v>242</v>
       </c>
     </row>
@@ -7974,12 +7974,15 @@
       <c r="C20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+      <c r="G20" t="s">
+        <v>231</v>
+      </c>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="9"/>
-      <c r="R20" s="9" t="s">
+      <c r="O20" s="8"/>
+      <c r="R20" s="8" t="s">
         <v>243</v>
       </c>
     </row>
@@ -7991,12 +7994,15 @@
       <c r="C21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
+      <c r="G21" t="s">
+        <v>231</v>
+      </c>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
       <c r="N21" s="4"/>
-      <c r="O21" s="9"/>
-      <c r="R21" s="9" t="s">
+      <c r="O21" s="8"/>
+      <c r="R21" s="8" t="s">
         <v>244</v>
       </c>
     </row>
@@ -8011,12 +8017,12 @@
       <c r="G22" t="s">
         <v>231</v>
       </c>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
       <c r="N22" s="4"/>
-      <c r="O22" s="9"/>
-      <c r="R22" s="9" t="s">
+      <c r="O22" s="8"/>
+      <c r="R22" s="8" t="s">
         <v>245</v>
       </c>
     </row>
@@ -8028,13 +8034,13 @@
       <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="10"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="12"/>
-      <c r="R23" s="9" t="s">
+      <c r="K23" s="9"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="11"/>
+      <c r="R23" s="8" t="s">
         <v>246</v>
       </c>
     </row>
@@ -8046,13 +8052,13 @@
       <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K24" s="10"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="14"/>
-      <c r="P24" s="12"/>
-      <c r="R24" s="9" t="s">
+      <c r="K24" s="9"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="11"/>
+      <c r="R24" s="8" t="s">
         <v>247</v>
       </c>
     </row>
@@ -8064,12 +8070,12 @@
       <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
       <c r="N25" s="4"/>
-      <c r="O25" s="9"/>
-      <c r="R25" s="9" t="s">
+      <c r="O25" s="8"/>
+      <c r="R25" s="8" t="s">
         <v>249</v>
       </c>
     </row>
@@ -8081,12 +8087,12 @@
       <c r="C26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
       <c r="N26" s="4"/>
-      <c r="O26" s="9"/>
-      <c r="R26" s="9" t="s">
+      <c r="O26" s="8"/>
+      <c r="R26" s="8" t="s">
         <v>250</v>
       </c>
     </row>
@@ -8098,12 +8104,12 @@
       <c r="C27" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
       <c r="N27" s="4"/>
-      <c r="O27" s="9"/>
-      <c r="R27" s="9" t="s">
+      <c r="O27" s="8"/>
+      <c r="R27" s="8" t="s">
         <v>251</v>
       </c>
     </row>
@@ -8115,12 +8121,12 @@
       <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="9"/>
-      <c r="R28" s="9" t="s">
+      <c r="O28" s="8"/>
+      <c r="R28" s="8" t="s">
         <v>252</v>
       </c>
     </row>
@@ -8132,12 +8138,12 @@
       <c r="C29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="9"/>
-      <c r="R29" s="9" t="s">
+      <c r="O29" s="8"/>
+      <c r="R29" s="8" t="s">
         <v>253</v>
       </c>
     </row>
@@ -8149,12 +8155,12 @@
       <c r="C30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="9"/>
-      <c r="R30" s="9" t="s">
+      <c r="O30" s="8"/>
+      <c r="R30" s="8" t="s">
         <v>254</v>
       </c>
     </row>
@@ -8166,12 +8172,12 @@
       <c r="C31" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
       <c r="N31" s="4"/>
-      <c r="O31" s="9"/>
-      <c r="R31" s="9" t="s">
+      <c r="O31" s="8"/>
+      <c r="R31" s="8" t="s">
         <v>255</v>
       </c>
     </row>
@@ -8183,12 +8189,12 @@
       <c r="C32" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="9"/>
-      <c r="R32" s="9" t="s">
+      <c r="O32" s="8"/>
+      <c r="R32" s="8" t="s">
         <v>256</v>
       </c>
     </row>
@@ -8200,12 +8206,12 @@
       <c r="C33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="9"/>
-      <c r="R33" s="9" t="s">
+      <c r="O33" s="8"/>
+      <c r="R33" s="8" t="s">
         <v>257</v>
       </c>
     </row>
@@ -8217,13 +8223,13 @@
       <c r="C34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K34" s="10"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="12"/>
-      <c r="R34" s="9" t="s">
+      <c r="K34" s="9"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="13"/>
+      <c r="P34" s="11"/>
+      <c r="R34" s="8" t="s">
         <v>258</v>
       </c>
     </row>
@@ -8235,13 +8241,13 @@
       <c r="C35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K35" s="10"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="12"/>
-      <c r="R35" s="9" t="s">
+      <c r="K35" s="9"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="13"/>
+      <c r="P35" s="11"/>
+      <c r="R35" s="8" t="s">
         <v>259</v>
       </c>
     </row>
@@ -8253,13 +8259,13 @@
       <c r="C36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K36" s="10"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="12"/>
-      <c r="R36" s="9" t="s">
+      <c r="K36" s="9"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="11"/>
+      <c r="R36" s="8" t="s">
         <v>261</v>
       </c>
     </row>
@@ -8271,12 +8277,12 @@
       <c r="C37" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
       <c r="N37" s="4"/>
-      <c r="O37" s="9"/>
-      <c r="R37" s="9" t="s">
+      <c r="O37" s="8"/>
+      <c r="R37" s="8" t="s">
         <v>262</v>
       </c>
     </row>
@@ -8288,12 +8294,12 @@
       <c r="C38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
       <c r="N38" s="4"/>
-      <c r="O38" s="9"/>
-      <c r="R38" s="9" t="s">
+      <c r="O38" s="8"/>
+      <c r="R38" s="8" t="s">
         <v>263</v>
       </c>
     </row>
@@ -8305,12 +8311,12 @@
       <c r="C39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
       <c r="N39" s="4"/>
-      <c r="O39" s="9"/>
-      <c r="R39" s="9" t="s">
+      <c r="O39" s="8"/>
+      <c r="R39" s="8" t="s">
         <v>260</v>
       </c>
     </row>
@@ -8322,12 +8328,12 @@
       <c r="C40" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
       <c r="N40" s="4"/>
-      <c r="O40" s="9"/>
-      <c r="R40" s="12" t="s">
+      <c r="O40" s="8"/>
+      <c r="R40" s="11" t="s">
         <v>248</v>
       </c>
     </row>
@@ -8339,12 +8345,12 @@
       <c r="C41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
       <c r="N41" s="4"/>
-      <c r="O41" s="9"/>
-      <c r="R41" s="12"/>
+      <c r="O41" s="8"/>
+      <c r="R41" s="11"/>
     </row>
     <row r="42" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
@@ -8354,12 +8360,12 @@
       <c r="C42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
       <c r="N42" s="4"/>
-      <c r="O42" s="9"/>
-      <c r="R42" s="12"/>
+      <c r="O42" s="8"/>
+      <c r="R42" s="11"/>
     </row>
     <row r="43" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
@@ -8369,12 +8375,12 @@
       <c r="C43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K43" s="10"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="12"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="11"/>
     </row>
     <row r="44" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -8384,12 +8390,12 @@
       <c r="C44" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K44" s="10"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="12"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="13"/>
+      <c r="P44" s="11"/>
     </row>
     <row r="45" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
@@ -8399,12 +8405,12 @@
       <c r="C45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K45" s="10"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="12"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="13"/>
+      <c r="P45" s="11"/>
     </row>
     <row r="46" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
@@ -8417,11 +8423,11 @@
       <c r="G46" t="s">
         <v>231</v>
       </c>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
       <c r="N46" s="4"/>
-      <c r="O46" s="9"/>
+      <c r="O46" s="8"/>
     </row>
     <row r="47" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
@@ -8431,11 +8437,11 @@
       <c r="C47" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
       <c r="N47" s="4"/>
-      <c r="O47" s="9"/>
+      <c r="O47" s="8"/>
     </row>
     <row r="48" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
@@ -8445,11 +8451,11 @@
       <c r="C48" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="9"/>
+      <c r="O48" s="8"/>
     </row>
     <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
@@ -8459,11 +8465,11 @@
       <c r="C49" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="9"/>
+      <c r="O49" s="8"/>
     </row>
     <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
@@ -8473,11 +8479,11 @@
       <c r="C50" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="K50" s="9"/>
-      <c r="L50" s="9"/>
-      <c r="M50" s="9"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="9"/>
+      <c r="O50" s="8"/>
     </row>
     <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
@@ -8487,11 +8493,11 @@
       <c r="C51" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="K51" s="9"/>
-      <c r="L51" s="9"/>
-      <c r="M51" s="9"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="9"/>
+      <c r="O51" s="8"/>
     </row>
     <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
@@ -8501,11 +8507,11 @@
       <c r="C52" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="K52" s="9"/>
-      <c r="L52" s="9"/>
-      <c r="M52" s="9"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="9"/>
+      <c r="O52" s="8"/>
     </row>
     <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
@@ -8515,11 +8521,11 @@
       <c r="C53" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="K53" s="9"/>
-      <c r="L53" s="9"/>
-      <c r="M53" s="9"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="9"/>
+      <c r="O53" s="8"/>
     </row>
     <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
@@ -8529,11 +8535,11 @@
       <c r="C54" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K54" s="9"/>
-      <c r="L54" s="9"/>
-      <c r="M54" s="9"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="9"/>
+      <c r="O54" s="8"/>
     </row>
     <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
@@ -8543,11 +8549,11 @@
       <c r="C55" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="K55" s="9"/>
-      <c r="L55" s="9"/>
-      <c r="M55" s="9"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="9"/>
+      <c r="O55" s="8"/>
     </row>
     <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
@@ -8557,11 +8563,11 @@
       <c r="C56" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
-      <c r="M56" s="9"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="9"/>
+      <c r="O56" s="8"/>
     </row>
     <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
@@ -8571,11 +8577,11 @@
       <c r="C57" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8"/>
       <c r="N57" s="4"/>
-      <c r="O57" s="9"/>
+      <c r="O57" s="8"/>
     </row>
     <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
@@ -8585,11 +8591,11 @@
       <c r="C58" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K58" s="9"/>
-      <c r="L58" s="9"/>
-      <c r="M58" s="9"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
       <c r="N58" s="4"/>
-      <c r="O58" s="9"/>
+      <c r="O58" s="8"/>
     </row>
     <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
@@ -8599,11 +8605,11 @@
       <c r="C59" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="K59" s="9"/>
-      <c r="L59" s="9"/>
-      <c r="M59" s="9"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8"/>
       <c r="N59" s="4"/>
-      <c r="O59" s="9"/>
+      <c r="O59" s="8"/>
     </row>
     <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
@@ -8613,11 +8619,11 @@
       <c r="C60" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="K60" s="9"/>
-      <c r="L60" s="9"/>
-      <c r="M60" s="9"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
       <c r="N60" s="4"/>
-      <c r="O60" s="9"/>
+      <c r="O60" s="8"/>
     </row>
     <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
@@ -8627,11 +8633,11 @@
       <c r="C61" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="K61" s="9"/>
-      <c r="L61" s="9"/>
-      <c r="M61" s="9"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8"/>
       <c r="N61" s="4"/>
-      <c r="O61" s="9"/>
+      <c r="O61" s="8"/>
     </row>
     <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
@@ -8641,11 +8647,11 @@
       <c r="C62" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="8"/>
+      <c r="M62" s="8"/>
       <c r="N62" s="4"/>
-      <c r="O62" s="9"/>
+      <c r="O62" s="8"/>
     </row>
     <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
@@ -8655,11 +8661,11 @@
       <c r="C63" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K63" s="9"/>
-      <c r="L63" s="9"/>
-      <c r="M63" s="9"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="8"/>
       <c r="N63" s="4"/>
-      <c r="O63" s="9"/>
+      <c r="O63" s="8"/>
     </row>
     <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
@@ -8669,11 +8675,11 @@
       <c r="C64" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="K64" s="9"/>
-      <c r="L64" s="9"/>
-      <c r="M64" s="9"/>
+      <c r="K64" s="8"/>
+      <c r="L64" s="8"/>
+      <c r="M64" s="8"/>
       <c r="N64" s="4"/>
-      <c r="O64" s="9"/>
+      <c r="O64" s="8"/>
     </row>
     <row r="65" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
@@ -8683,11 +8689,11 @@
       <c r="C65" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="K65" s="9"/>
-      <c r="L65" s="9"/>
-      <c r="M65" s="9"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+      <c r="M65" s="8"/>
       <c r="N65" s="4"/>
-      <c r="O65" s="9"/>
+      <c r="O65" s="8"/>
     </row>
     <row r="66" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
@@ -8697,11 +8703,11 @@
       <c r="C66" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="K66" s="9"/>
-      <c r="L66" s="9"/>
-      <c r="M66" s="9"/>
+      <c r="K66" s="8"/>
+      <c r="L66" s="8"/>
+      <c r="M66" s="8"/>
       <c r="N66" s="4"/>
-      <c r="O66" s="9"/>
+      <c r="O66" s="8"/>
     </row>
     <row r="67" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
@@ -8711,11 +8717,11 @@
       <c r="C67" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="K67" s="9"/>
-      <c r="L67" s="9"/>
-      <c r="M67" s="9"/>
+      <c r="K67" s="8"/>
+      <c r="L67" s="8"/>
+      <c r="M67" s="8"/>
       <c r="N67" s="4"/>
-      <c r="O67" s="9"/>
+      <c r="O67" s="8"/>
     </row>
     <row r="68" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
@@ -8725,11 +8731,11 @@
       <c r="C68" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K68" s="9"/>
-      <c r="L68" s="9"/>
-      <c r="M68" s="9"/>
+      <c r="K68" s="8"/>
+      <c r="L68" s="8"/>
+      <c r="M68" s="8"/>
       <c r="N68" s="4"/>
-      <c r="O68" s="9"/>
+      <c r="O68" s="8"/>
     </row>
     <row r="69" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
@@ -8739,11 +8745,11 @@
       <c r="C69" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="K69" s="9"/>
-      <c r="L69" s="9"/>
-      <c r="M69" s="9"/>
+      <c r="K69" s="8"/>
+      <c r="L69" s="8"/>
+      <c r="M69" s="8"/>
       <c r="N69" s="4"/>
-      <c r="O69" s="9"/>
+      <c r="O69" s="8"/>
     </row>
     <row r="70" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
@@ -8753,11 +8759,11 @@
       <c r="C70" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="K70" s="9"/>
-      <c r="L70" s="9"/>
-      <c r="M70" s="9"/>
+      <c r="K70" s="8"/>
+      <c r="L70" s="8"/>
+      <c r="M70" s="8"/>
       <c r="N70" s="4"/>
-      <c r="O70" s="9"/>
+      <c r="O70" s="8"/>
     </row>
     <row r="71" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
@@ -8767,12 +8773,12 @@
       <c r="C71" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="K71" s="10"/>
-      <c r="L71" s="12"/>
-      <c r="M71" s="12"/>
-      <c r="N71" s="12"/>
-      <c r="O71" s="14"/>
-      <c r="P71" s="12"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="11"/>
+      <c r="M71" s="11"/>
+      <c r="N71" s="11"/>
+      <c r="O71" s="13"/>
+      <c r="P71" s="11"/>
     </row>
     <row r="72" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
@@ -8782,12 +8788,12 @@
       <c r="C72" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="K72" s="10"/>
-      <c r="L72" s="12"/>
-      <c r="M72" s="12"/>
-      <c r="N72" s="12"/>
-      <c r="O72" s="14"/>
-      <c r="P72" s="12"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="11"/>
+      <c r="M72" s="11"/>
+      <c r="N72" s="11"/>
+      <c r="O72" s="13"/>
+      <c r="P72" s="11"/>
     </row>
     <row r="73" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
@@ -8797,12 +8803,12 @@
       <c r="C73" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="K73" s="10"/>
-      <c r="L73" s="12"/>
-      <c r="M73" s="12"/>
-      <c r="N73" s="12"/>
-      <c r="O73" s="14"/>
-      <c r="P73" s="12"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="11"/>
+      <c r="M73" s="11"/>
+      <c r="N73" s="11"/>
+      <c r="O73" s="13"/>
+      <c r="P73" s="11"/>
     </row>
     <row r="74" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
@@ -8812,11 +8818,11 @@
       <c r="C74" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="K74" s="9"/>
-      <c r="L74" s="9"/>
-      <c r="M74" s="9"/>
+      <c r="K74" s="8"/>
+      <c r="L74" s="8"/>
+      <c r="M74" s="8"/>
       <c r="N74" s="4"/>
-      <c r="O74" s="9"/>
+      <c r="O74" s="8"/>
     </row>
     <row r="75" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
@@ -8826,11 +8832,11 @@
       <c r="C75" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="K75" s="9"/>
-      <c r="L75" s="9"/>
-      <c r="M75" s="9"/>
+      <c r="K75" s="8"/>
+      <c r="L75" s="8"/>
+      <c r="M75" s="8"/>
       <c r="N75" s="4"/>
-      <c r="O75" s="9"/>
+      <c r="O75" s="8"/>
     </row>
     <row r="76" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
@@ -8840,11 +8846,11 @@
       <c r="C76" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="K76" s="9"/>
-      <c r="L76" s="9"/>
-      <c r="M76" s="9"/>
+      <c r="K76" s="8"/>
+      <c r="L76" s="8"/>
+      <c r="M76" s="8"/>
       <c r="N76" s="4"/>
-      <c r="O76" s="9"/>
+      <c r="O76" s="8"/>
     </row>
     <row r="77" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
@@ -8854,11 +8860,11 @@
       <c r="C77" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9"/>
-      <c r="M77" s="9"/>
+      <c r="K77" s="8"/>
+      <c r="L77" s="8"/>
+      <c r="M77" s="8"/>
       <c r="N77" s="4"/>
-      <c r="O77" s="9"/>
+      <c r="O77" s="8"/>
     </row>
     <row r="78" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
@@ -8868,11 +8874,11 @@
       <c r="C78" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="K78" s="9"/>
-      <c r="L78" s="9"/>
-      <c r="M78" s="9"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="8"/>
+      <c r="M78" s="8"/>
       <c r="N78" s="4"/>
-      <c r="O78" s="9"/>
+      <c r="O78" s="8"/>
     </row>
     <row r="79" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
@@ -8882,172 +8888,172 @@
       <c r="C79" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="K79" s="10"/>
-      <c r="L79" s="12"/>
-      <c r="M79" s="12"/>
-      <c r="N79" s="12"/>
-      <c r="O79" s="12"/>
-      <c r="P79" s="12"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="11"/>
+      <c r="M79" s="11"/>
+      <c r="N79" s="11"/>
+      <c r="O79" s="11"/>
+      <c r="P79" s="11"/>
     </row>
     <row r="80" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K80" s="10"/>
-      <c r="L80" s="12"/>
-      <c r="M80" s="12"/>
-      <c r="N80" s="12"/>
-      <c r="O80" s="12"/>
-      <c r="P80" s="12"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="11"/>
+      <c r="M80" s="11"/>
+      <c r="N80" s="11"/>
+      <c r="O80" s="11"/>
+      <c r="P80" s="11"/>
     </row>
     <row r="81" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K81" s="10"/>
-      <c r="L81" s="12"/>
-      <c r="M81" s="12"/>
-      <c r="N81" s="12"/>
-      <c r="O81" s="12"/>
-      <c r="P81" s="12"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="11"/>
+      <c r="M81" s="11"/>
+      <c r="N81" s="11"/>
+      <c r="O81" s="11"/>
+      <c r="P81" s="11"/>
     </row>
     <row r="82" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K82" s="9"/>
-      <c r="L82" s="9"/>
-      <c r="M82" s="9"/>
-      <c r="N82" s="9"/>
-      <c r="O82" s="9"/>
+      <c r="K82" s="8"/>
+      <c r="L82" s="8"/>
+      <c r="M82" s="8"/>
+      <c r="N82" s="8"/>
+      <c r="O82" s="8"/>
     </row>
     <row r="83" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K83" s="9"/>
-      <c r="L83" s="9"/>
-      <c r="M83" s="9"/>
-      <c r="N83" s="9"/>
-      <c r="O83" s="9"/>
+      <c r="K83" s="8"/>
+      <c r="L83" s="8"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="8"/>
+      <c r="O83" s="8"/>
     </row>
     <row r="84" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="2"/>
       <c r="C84" s="1"/>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
-      <c r="M84" s="9"/>
-      <c r="N84" s="9"/>
-      <c r="O84" s="9"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="8"/>
+      <c r="N84" s="8"/>
+      <c r="O84" s="8"/>
     </row>
     <row r="85" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="2"/>
       <c r="C85" s="1"/>
-      <c r="K85" s="9"/>
-      <c r="L85" s="9"/>
-      <c r="M85" s="9"/>
-      <c r="N85" s="9"/>
-      <c r="O85" s="9"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="8"/>
+      <c r="O85" s="8"/>
     </row>
     <row r="86" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="2"/>
       <c r="C86" s="1"/>
-      <c r="K86" s="9"/>
-      <c r="L86" s="9"/>
-      <c r="M86" s="9"/>
-      <c r="N86" s="9"/>
-      <c r="O86" s="9"/>
+      <c r="K86" s="8"/>
+      <c r="L86" s="8"/>
+      <c r="M86" s="8"/>
+      <c r="N86" s="8"/>
+      <c r="O86" s="8"/>
     </row>
     <row r="87" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K87" s="9"/>
-      <c r="L87" s="9"/>
-      <c r="M87" s="9"/>
-      <c r="N87" s="9"/>
-      <c r="O87" s="9"/>
+      <c r="K87" s="8"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="8"/>
+      <c r="N87" s="8"/>
+      <c r="O87" s="8"/>
     </row>
     <row r="88" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K88" s="9"/>
-      <c r="L88" s="9"/>
-      <c r="M88" s="9"/>
-      <c r="N88" s="9"/>
-      <c r="O88" s="9"/>
+      <c r="K88" s="8"/>
+      <c r="L88" s="8"/>
+      <c r="M88" s="8"/>
+      <c r="N88" s="8"/>
+      <c r="O88" s="8"/>
     </row>
     <row r="89" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K89" s="9"/>
-      <c r="L89" s="9"/>
-      <c r="M89" s="9"/>
-      <c r="N89" s="9"/>
-      <c r="O89" s="9"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="8"/>
+      <c r="N89" s="8"/>
+      <c r="O89" s="8"/>
     </row>
     <row r="90" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K90" s="9"/>
-      <c r="L90" s="9"/>
-      <c r="M90" s="9"/>
-      <c r="N90" s="9"/>
-      <c r="O90" s="9"/>
+      <c r="K90" s="8"/>
+      <c r="L90" s="8"/>
+      <c r="M90" s="8"/>
+      <c r="N90" s="8"/>
+      <c r="O90" s="8"/>
     </row>
     <row r="91" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K91" s="9"/>
-      <c r="L91" s="9"/>
-      <c r="M91" s="9"/>
-      <c r="N91" s="9"/>
-      <c r="O91" s="9"/>
+      <c r="K91" s="8"/>
+      <c r="L91" s="8"/>
+      <c r="M91" s="8"/>
+      <c r="N91" s="8"/>
+      <c r="O91" s="8"/>
     </row>
     <row r="92" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K92" s="9"/>
-      <c r="L92" s="9"/>
-      <c r="M92" s="9"/>
-      <c r="N92" s="9"/>
-      <c r="O92" s="9"/>
+      <c r="K92" s="8"/>
+      <c r="L92" s="8"/>
+      <c r="M92" s="8"/>
+      <c r="N92" s="8"/>
+      <c r="O92" s="8"/>
     </row>
     <row r="93" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K93" s="9"/>
-      <c r="L93" s="9"/>
-      <c r="M93" s="9"/>
-      <c r="N93" s="9"/>
-      <c r="O93" s="9"/>
+      <c r="K93" s="8"/>
+      <c r="L93" s="8"/>
+      <c r="M93" s="8"/>
+      <c r="N93" s="8"/>
+      <c r="O93" s="8"/>
     </row>
     <row r="94" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K94" s="9"/>
-      <c r="L94" s="9"/>
-      <c r="M94" s="9"/>
-      <c r="N94" s="9"/>
-      <c r="O94" s="9"/>
+      <c r="K94" s="8"/>
+      <c r="L94" s="8"/>
+      <c r="M94" s="8"/>
+      <c r="N94" s="8"/>
+      <c r="O94" s="8"/>
     </row>
     <row r="95" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="2"/>
       <c r="C95" s="1"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="9"/>
-      <c r="M95" s="9"/>
-      <c r="N95" s="9"/>
-      <c r="O95" s="9"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="8"/>
+      <c r="N95" s="8"/>
+      <c r="O95" s="8"/>
     </row>
     <row r="96" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="2"/>
       <c r="C96" s="1"/>
-      <c r="K96" s="9"/>
-      <c r="L96" s="9"/>
-      <c r="M96" s="9"/>
-      <c r="N96" s="9"/>
-      <c r="O96" s="9"/>
+      <c r="K96" s="8"/>
+      <c r="L96" s="8"/>
+      <c r="M96" s="8"/>
+      <c r="N96" s="8"/>
+      <c r="O96" s="8"/>
     </row>
     <row r="97" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="2"/>
       <c r="C97" s="1"/>
-      <c r="K97" s="9"/>
-      <c r="L97" s="9"/>
-      <c r="M97" s="9"/>
-      <c r="N97" s="9"/>
-      <c r="O97" s="9"/>
+      <c r="K97" s="8"/>
+      <c r="L97" s="8"/>
+      <c r="M97" s="8"/>
+      <c r="N97" s="8"/>
+      <c r="O97" s="8"/>
     </row>
     <row r="98" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
-      <c r="M98" s="9"/>
-      <c r="N98" s="9"/>
-      <c r="O98" s="9"/>
+      <c r="K98" s="8"/>
+      <c r="L98" s="8"/>
+      <c r="M98" s="8"/>
+      <c r="N98" s="8"/>
+      <c r="O98" s="8"/>
     </row>
     <row r="99" spans="1:16" ht="18" x14ac:dyDescent="0.2">
-      <c r="K99" s="9"/>
-      <c r="L99" s="9"/>
-      <c r="M99" s="9"/>
-      <c r="N99" s="9"/>
-      <c r="O99" s="9"/>
+      <c r="K99" s="8"/>
+      <c r="L99" s="8"/>
+      <c r="M99" s="8"/>
+      <c r="N99" s="8"/>
+      <c r="O99" s="8"/>
     </row>
     <row r="100" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
@@ -9057,11 +9063,11 @@
       <c r="C100" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K100" s="9"/>
-      <c r="L100" s="9"/>
-      <c r="M100" s="9"/>
-      <c r="N100" s="9"/>
-      <c r="O100" s="9"/>
+      <c r="K100" s="8"/>
+      <c r="L100" s="8"/>
+      <c r="M100" s="8"/>
+      <c r="N100" s="8"/>
+      <c r="O100" s="8"/>
     </row>
     <row r="101" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
@@ -9071,11 +9077,11 @@
       <c r="C101" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K101" s="9"/>
-      <c r="L101" s="9"/>
-      <c r="M101" s="9"/>
-      <c r="N101" s="9"/>
-      <c r="O101" s="9"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="8"/>
+      <c r="N101" s="8"/>
+      <c r="O101" s="8"/>
     </row>
     <row r="102" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
@@ -9085,11 +9091,11 @@
       <c r="C102" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K102" s="9"/>
-      <c r="L102" s="9"/>
-      <c r="M102" s="9"/>
-      <c r="N102" s="9"/>
-      <c r="O102" s="9"/>
+      <c r="K102" s="8"/>
+      <c r="L102" s="8"/>
+      <c r="M102" s="8"/>
+      <c r="N102" s="8"/>
+      <c r="O102" s="8"/>
     </row>
     <row r="103" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
@@ -9099,11 +9105,11 @@
       <c r="C103" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K103" s="9"/>
-      <c r="L103" s="9"/>
-      <c r="M103" s="9"/>
-      <c r="N103" s="9"/>
-      <c r="O103" s="9"/>
+      <c r="K103" s="8"/>
+      <c r="L103" s="8"/>
+      <c r="M103" s="8"/>
+      <c r="N103" s="8"/>
+      <c r="O103" s="8"/>
     </row>
     <row r="104" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
@@ -9113,11 +9119,11 @@
       <c r="C104" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
-      <c r="M104" s="9"/>
-      <c r="N104" s="9"/>
-      <c r="O104" s="9"/>
+      <c r="K104" s="8"/>
+      <c r="L104" s="8"/>
+      <c r="M104" s="8"/>
+      <c r="N104" s="8"/>
+      <c r="O104" s="8"/>
     </row>
     <row r="105" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
@@ -9127,43 +9133,43 @@
       <c r="C105" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K105" s="9"/>
-      <c r="L105" s="9"/>
-      <c r="M105" s="9"/>
-      <c r="N105" s="9"/>
-      <c r="O105" s="9"/>
+      <c r="K105" s="8"/>
+      <c r="L105" s="8"/>
+      <c r="M105" s="8"/>
+      <c r="N105" s="8"/>
+      <c r="O105" s="8"/>
     </row>
     <row r="106" spans="1:16" ht="22" x14ac:dyDescent="0.3">
       <c r="B106" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="K106" s="9"/>
-      <c r="L106" s="9"/>
-      <c r="M106" s="9"/>
-      <c r="N106" s="9"/>
-      <c r="O106" s="9"/>
+      <c r="K106" s="8"/>
+      <c r="L106" s="8"/>
+      <c r="M106" s="8"/>
+      <c r="N106" s="8"/>
+      <c r="O106" s="8"/>
     </row>
     <row r="107" spans="1:16" ht="22" x14ac:dyDescent="0.3">
       <c r="B107" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="K107" s="10"/>
-      <c r="L107" s="12"/>
-      <c r="M107" s="12"/>
-      <c r="N107" s="12"/>
-      <c r="O107" s="14"/>
-      <c r="P107" s="12"/>
+      <c r="K107" s="9"/>
+      <c r="L107" s="11"/>
+      <c r="M107" s="11"/>
+      <c r="N107" s="11"/>
+      <c r="O107" s="13"/>
+      <c r="P107" s="11"/>
     </row>
     <row r="108" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K108" s="10"/>
-      <c r="L108" s="12"/>
-      <c r="M108" s="12"/>
-      <c r="N108" s="12"/>
-      <c r="O108" s="14"/>
-      <c r="P108" s="12"/>
+      <c r="K108" s="9"/>
+      <c r="L108" s="11"/>
+      <c r="M108" s="11"/>
+      <c r="N108" s="11"/>
+      <c r="O108" s="13"/>
+      <c r="P108" s="11"/>
     </row>
     <row r="109" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
@@ -9173,12 +9179,12 @@
       <c r="C109" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="K109" s="10"/>
-      <c r="L109" s="12"/>
-      <c r="M109" s="12"/>
-      <c r="N109" s="12"/>
-      <c r="O109" s="14"/>
-      <c r="P109" s="12"/>
+      <c r="K109" s="9"/>
+      <c r="L109" s="11"/>
+      <c r="M109" s="11"/>
+      <c r="N109" s="11"/>
+      <c r="O109" s="13"/>
+      <c r="P109" s="11"/>
     </row>
     <row r="110" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
@@ -9188,11 +9194,11 @@
       <c r="C110" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K110" s="9"/>
-      <c r="L110" s="9"/>
-      <c r="M110" s="9"/>
+      <c r="K110" s="8"/>
+      <c r="L110" s="8"/>
+      <c r="M110" s="8"/>
       <c r="N110" s="4"/>
-      <c r="O110" s="9"/>
+      <c r="O110" s="8"/>
     </row>
     <row r="111" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
@@ -9202,11 +9208,11 @@
       <c r="C111" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K111" s="9"/>
-      <c r="L111" s="9"/>
-      <c r="M111" s="9"/>
+      <c r="K111" s="8"/>
+      <c r="L111" s="8"/>
+      <c r="M111" s="8"/>
       <c r="N111" s="4"/>
-      <c r="O111" s="9"/>
+      <c r="O111" s="8"/>
     </row>
     <row r="112" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
@@ -9216,11 +9222,11 @@
       <c r="C112" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K112" s="9"/>
-      <c r="L112" s="9"/>
-      <c r="M112" s="9"/>
+      <c r="K112" s="8"/>
+      <c r="L112" s="8"/>
+      <c r="M112" s="8"/>
       <c r="N112" s="4"/>
-      <c r="O112" s="9"/>
+      <c r="O112" s="8"/>
     </row>
     <row r="113" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
@@ -9253,12 +9259,12 @@
       <c r="C116" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E116" s="7" t="s">
+      <c r="E116" s="14" t="s">
         <v>230</v>
       </c>
-      <c r="F116" s="7"/>
-      <c r="G116" s="7"/>
-      <c r="H116" s="7"/>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
+      <c r="H116" s="14"/>
     </row>
     <row r="117" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>

</xml_diff>

<commit_message>
First commit for <ding> feature>
</commit_message>
<xml_diff>
--- a/emoList.xlsx
+++ b/emoList.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="266">
   <si>
     <t>:)</t>
   </si>
@@ -822,13 +822,19 @@
   </si>
   <si>
     <t>~</t>
+  </si>
+  <si>
+    <t>&lt;ding&gt;</t>
+  </si>
+  <si>
+    <t>BUZZ!!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -895,6 +901,13 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -917,7 +930,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -935,6 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7636,10 +7650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R137"/>
+  <dimension ref="A1:R138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="F127" sqref="F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9453,6 +9467,14 @@
       </c>
       <c r="C137" s="5" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A138" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change queue shift to pop
</commit_message>
<xml_diff>
--- a/emoList.xlsx
+++ b/emoList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27204"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="271">
   <si>
     <t>:)</t>
   </si>
@@ -822,6 +822,27 @@
   </si>
   <si>
     <t>~</t>
+  </si>
+  <si>
+    <t>/:-)</t>
+  </si>
+  <si>
+    <t>X-(</t>
+  </si>
+  <si>
+    <t>O:)</t>
+  </si>
+  <si>
+    <t>:b</t>
+  </si>
+  <si>
+    <t>:@</t>
+  </si>
+  <si>
+    <t>:$</t>
+  </si>
+  <si>
+    <t>FIX no :&lt;</t>
   </si>
 </sst>
 </file>
@@ -7638,8 +7659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7772,6 +7793,9 @@
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I9" t="s">
+        <v>269</v>
+      </c>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -7863,6 +7887,12 @@
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="H14" t="s">
+        <v>265</v>
+      </c>
+      <c r="I14" t="s">
+        <v>268</v>
+      </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
@@ -8033,6 +8063,9 @@
       </c>
       <c r="C23" s="1" t="s">
         <v>45</v>
+      </c>
+      <c r="H23" t="s">
+        <v>264</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="11"/>
@@ -8070,6 +8103,9 @@
       <c r="C25" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="H25" t="s">
+        <v>266</v>
+      </c>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
@@ -8086,6 +8122,9 @@
       </c>
       <c r="C26" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="H26" t="s">
+        <v>267</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -8422,6 +8461,9 @@
       </c>
       <c r="G46" t="s">
         <v>231</v>
+      </c>
+      <c r="H46" t="s">
+        <v>270</v>
       </c>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>

</xml_diff>

<commit_message>
add buzz to list
</commit_message>
<xml_diff>
--- a/emoList.xlsx
+++ b/emoList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27204"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27217"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="273">
   <si>
     <t>:)</t>
   </si>
@@ -843,13 +843,19 @@
   </si>
   <si>
     <t>FIX no :&lt;</t>
+  </si>
+  <si>
+    <t>BUZZ!!!</t>
+  </si>
+  <si>
+    <t>&lt;ding&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -916,6 +922,13 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -938,7 +951,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -956,6 +969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7657,10 +7671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R137"/>
+  <dimension ref="A1:R138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9495,6 +9509,14 @@
       </c>
       <c r="C137" s="5" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A138" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first commit, remove everything, change emoticons to obj json, using storage
</commit_message>
<xml_diff>
--- a/emoList.xlsx
+++ b/emoList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27217"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="271">
   <si>
     <t>:)</t>
   </si>
@@ -728,9 +728,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>cant</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -845,10 +842,7 @@
     <t>FIX no :&lt;</t>
   </si>
   <si>
-    <t>BUZZ!!!</t>
-  </si>
-  <si>
-    <t>&lt;ding&gt;</t>
+    <t>x cant</t>
   </si>
 </sst>
 </file>
@@ -966,10 +960,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7673,8 +7667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7773,7 +7767,7 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>232</v>
+        <v>270</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="11"/>
@@ -7808,7 +7802,7 @@
         <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
@@ -7833,7 +7827,7 @@
       <c r="N10" s="10"/>
       <c r="O10" s="8"/>
       <c r="R10" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -7853,7 +7847,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="8"/>
       <c r="R11" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -7870,7 +7864,7 @@
       <c r="N12" s="4"/>
       <c r="O12" s="8"/>
       <c r="R12" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -7890,7 +7884,7 @@
       <c r="N13" s="4"/>
       <c r="O13" s="8"/>
       <c r="R13" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -7902,10 +7896,10 @@
         <v>27</v>
       </c>
       <c r="H14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -7913,7 +7907,7 @@
       <c r="N14" s="4"/>
       <c r="O14" s="8"/>
       <c r="R14" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -7933,7 +7927,7 @@
       <c r="N15" s="4"/>
       <c r="O15" s="8"/>
       <c r="R15" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -7953,7 +7947,7 @@
       <c r="N16" s="4"/>
       <c r="O16" s="8"/>
       <c r="R16" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -7973,7 +7967,7 @@
       <c r="N17" s="4"/>
       <c r="O17" s="8"/>
       <c r="R17" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -7990,7 +7984,7 @@
       <c r="N18" s="4"/>
       <c r="O18" s="8"/>
       <c r="R18" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8007,7 +8001,7 @@
       <c r="N19" s="4"/>
       <c r="O19" s="8"/>
       <c r="R19" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8027,7 +8021,7 @@
       <c r="N20" s="4"/>
       <c r="O20" s="8"/>
       <c r="R20" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8047,7 +8041,7 @@
       <c r="N21" s="4"/>
       <c r="O21" s="8"/>
       <c r="R21" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8067,7 +8061,7 @@
       <c r="N22" s="4"/>
       <c r="O22" s="8"/>
       <c r="R22" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8079,7 +8073,7 @@
         <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="11"/>
@@ -8088,7 +8082,7 @@
       <c r="O23" s="13"/>
       <c r="P23" s="11"/>
       <c r="R23" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8106,7 +8100,7 @@
       <c r="O24" s="13"/>
       <c r="P24" s="11"/>
       <c r="R24" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8118,7 +8112,7 @@
         <v>49</v>
       </c>
       <c r="H25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
@@ -8126,7 +8120,7 @@
       <c r="N25" s="4"/>
       <c r="O25" s="8"/>
       <c r="R25" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8138,7 +8132,7 @@
         <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -8146,7 +8140,7 @@
       <c r="N26" s="4"/>
       <c r="O26" s="8"/>
       <c r="R26" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8163,7 +8157,7 @@
       <c r="N27" s="4"/>
       <c r="O27" s="8"/>
       <c r="R27" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8180,7 +8174,7 @@
       <c r="N28" s="4"/>
       <c r="O28" s="8"/>
       <c r="R28" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8197,7 +8191,7 @@
       <c r="N29" s="4"/>
       <c r="O29" s="8"/>
       <c r="R29" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8214,7 +8208,7 @@
       <c r="N30" s="4"/>
       <c r="O30" s="8"/>
       <c r="R30" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8231,7 +8225,7 @@
       <c r="N31" s="4"/>
       <c r="O31" s="8"/>
       <c r="R31" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8248,7 +8242,7 @@
       <c r="N32" s="4"/>
       <c r="O32" s="8"/>
       <c r="R32" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8265,7 +8259,7 @@
       <c r="N33" s="4"/>
       <c r="O33" s="8"/>
       <c r="R33" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8283,7 +8277,7 @@
       <c r="O34" s="13"/>
       <c r="P34" s="11"/>
       <c r="R34" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8301,7 +8295,7 @@
       <c r="O35" s="13"/>
       <c r="P35" s="11"/>
       <c r="R35" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8319,7 +8313,7 @@
       <c r="O36" s="13"/>
       <c r="P36" s="11"/>
       <c r="R36" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8336,7 +8330,7 @@
       <c r="N37" s="4"/>
       <c r="O37" s="8"/>
       <c r="R37" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8353,7 +8347,7 @@
       <c r="N38" s="4"/>
       <c r="O38" s="8"/>
       <c r="R38" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8370,7 +8364,7 @@
       <c r="N39" s="4"/>
       <c r="O39" s="8"/>
       <c r="R39" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8387,7 +8381,7 @@
       <c r="N40" s="4"/>
       <c r="O40" s="8"/>
       <c r="R40" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="21" x14ac:dyDescent="0.25">
@@ -8477,7 +8471,7 @@
         <v>231</v>
       </c>
       <c r="H46" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
@@ -9315,12 +9309,12 @@
       <c r="C116" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="E116" s="14" t="s">
+      <c r="E116" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="F116" s="14"/>
-      <c r="G116" s="14"/>
-      <c r="H116" s="14"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="15"/>
+      <c r="H116" s="15"/>
     </row>
     <row r="117" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
@@ -9512,12 +9506,8 @@
       </c>
     </row>
     <row r="138" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="A138" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="B138" s="6" t="s">
-        <v>272</v>
-      </c>
+      <c r="A138" s="14"/>
+      <c r="B138" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="G1:G137"/>

</xml_diff>